<commit_message>
Testplan under utvikling + status ok
</commit_message>
<xml_diff>
--- a/Testplan.xlsx
+++ b/Testplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haako\Documents\Clench-mouthguard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C044B21-5BF6-434B-9227-9B1BB470D49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10167648-7CBF-411B-8E4A-B46D55E2C282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="1" xr2:uid="{9043C907-DEA0-436E-8321-8E2700439155}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{9043C907-DEA0-436E-8321-8E2700439155}"/>
   </bookViews>
   <sheets>
     <sheet name="Referanse" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
   <si>
     <t>Package / Type</t>
   </si>
@@ -79,27 +79,6 @@
     <t>Typical use / notes</t>
   </si>
   <si>
-    <t>Wrist‑based health sensor band reference platform lastminuteengineers​</t>
-  </si>
-  <si>
-    <t>SpO₂, heart rate (HR), heart rate variability (HRV) health‑sensor platform</t>
-  </si>
-  <si>
-    <t>MAX20303 PMIC, MAX32664C biometric sensor hub, MAX86174A AFE for PPG lastminuteengineers​</t>
-  </si>
-  <si>
-    <t>On‑board PMIC from battery/USB lastminuteengineers​</t>
-  </si>
-  <si>
-    <t>Bluetooth to Android app or PC GUI lastminuteengineers​</t>
-  </si>
-  <si>
-    <t>Micro board, sensor board, MAXDAP‑TYPE‑C board, enclosure/straps, hardware design files, firmware lastminuteengineers​</t>
-  </si>
-  <si>
-    <t>Complete wrist‑worn platform for remote patient monitoring lastminuteengineers​</t>
-  </si>
-  <si>
     <t>MAX30110ACCEVKIT#</t>
   </si>
   <si>
@@ -169,47 +148,104 @@
     <t>Module (LEDs + PD + AFE + ADC) farnell+1</t>
   </si>
   <si>
-    <t>Pulse oximeter (SpO₂) and heart‑rate sensing farnell+1</t>
-  </si>
-  <si>
-    <t>Integrated MAX30102 farnell+1</t>
-  </si>
-  <si>
-    <t>1.8 V logic + 3.3 V LED supply (modules: 3.3–5 V) farnell+1</t>
-  </si>
-  <si>
-    <t>I²C farnell+1</t>
-  </si>
-  <si>
-    <t>Integrated HR/SpO₂ sensor, 18‑bit ADC, 32‑sample FIFO farnell+1</t>
-  </si>
-  <si>
-    <t>Module (LEDs + PD + AFE + ADC) lastminuteengineers+2</t>
-  </si>
-  <si>
-    <t>Pulse oximeter (SpO₂) and heart‑rate sensing lastminuteengineers+1</t>
-  </si>
-  <si>
-    <t>Integrated MAX30100 lastminuteengineers+1</t>
-  </si>
-  <si>
-    <t>1.8 V core + 3.3 V LED (modules: 3.3–5 V) lastminuteengineers+1</t>
-  </si>
-  <si>
-    <t>I²C lastminuteengineers+1</t>
-  </si>
-  <si>
-    <t>Older HR/SpO₂ sensor, 16‑bit ADC, 16‑sample FIFO easyelecmodule+1</t>
-  </si>
-  <si>
     <t>Hvor er denne montro?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I²C </t>
+  </si>
+  <si>
+    <t>Integrated HR/SpO₂ sensor, 18‑bit ADC, 32‑sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Older HR/SpO₂ sensor, 16‑bit ADC, 16‑sample FIFO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.8 V core + 3.3 V LED (modules: 3.3–5 V) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrated MAX30100 </t>
+  </si>
+  <si>
+    <t>Module (LEDs + PD + AFE + ADC)</t>
+  </si>
+  <si>
+    <t>Pulse oximeter (SpO₂) and heart‑rate sensing . It integrates a red LED and an infrared LED, a photodetector, optical components, and low-noise electronic circuits with ambient light suppression.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The MAX30102 operates with a 1.8V power supply and an independent 5.0V power supply for the internal LED, and is applied to wearable devices for heart rate and blood oxygen collection and detection, </t>
+  </si>
+  <si>
+    <t>Integrated MAX30102</t>
+  </si>
+  <si>
+    <t>MAX30110</t>
+  </si>
+  <si>
+    <t>MAX30112</t>
+  </si>
+  <si>
+    <t>2.8mm x 2.0mm, 24-bump WLP (6x4, 0.4mm pitch) ​</t>
+  </si>
+  <si>
+    <t>Integrated optical AFE with 19-bit sigma-delta ADC, ambient light cancellation, two LED drivers (up to 200mA), 32-sample FIFO for pulse oximetry (SpO2), heart rate (HR), HR variability </t>
+  </si>
+  <si>
+    <t>MAX30110 (Analog Devices/Maxim Integrated) ​</t>
+  </si>
+  <si>
+    <t>1.8V (VDD_ANA/VDD_DIG), 3.1V–5.25V (VLED for LEDs) </t>
+  </si>
+  <si>
+    <t>SPI (up to 4MHz), optional FCLK input </t>
+  </si>
+  <si>
+    <t>EV kit: MAX30110ACCEVKIT# with main board, sensor daughter boards (e.g., SFH7050), USB-powered ​</t>
+  </si>
+  <si>
+    <t>Wrist/in-ear wearables, fitness trackers, SpO2/HR monitoring; ultra-low power (&lt;25μA at 25sps), -40°C to +85°C </t>
+  </si>
+  <si>
+    <t>MAX30112 (Analog Devices/Maxim Integrated) ​</t>
+  </si>
+  <si>
+    <t>I²C (up to 400kHz), optional FCLK input </t>
+  </si>
+  <si>
+    <t>Shares MAX30110ACCEVKIT# with main board, sensor daughter boards ​</t>
+  </si>
+  <si>
+    <t>MAX20303 PMIC, MAX32664C biometric sensor hub, MAX86174A AFE for PPG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bluetooth to Android app or PC GUI </t>
+  </si>
+  <si>
+    <t>PPG optical heart-rate sensor (green/red/IR LEDs, 2 photodiodes), SpO2/HR/HRV/respiration/sleep quality algorithms, 3-axis IMU (accel/gyro) </t>
+  </si>
+  <si>
+    <t>On‑board PMIC from battery/USB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Micro board, sensor board, MAXDAP‑TYPE‑C board, enclosure/straps, hardware design files, firmware </t>
+  </si>
+  <si>
+    <t>Complete wrist‑worn platform for remote patient monitoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wrist‑based health sensor band reference platform </t>
+  </si>
+  <si>
+    <t>Modus</t>
+  </si>
+  <si>
+    <t>Filament -&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +286,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.6"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -278,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -301,7 +353,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
@@ -332,8 +389,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>146194</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>97301</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114110</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -496,8 +553,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>733953</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>404</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1263719</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -530,6 +587,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>966338</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>81287</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Bilde 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79E1E1CD-8829-E2EA-9994-D6BF7B0D6188}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="85725" y="3514725"/>
+          <a:ext cx="1642613" cy="1257626"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>205037</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171951</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1126911</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>105647</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Bilde 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{577CCED6-B256-A51B-F490-6E0D292407DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="205037" y="7034965"/>
+          <a:ext cx="3268032" cy="2640801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -537,16 +682,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>537483</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>299358</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>319122</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>146198</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>80997</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>117623</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -569,8 +714,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8919483" y="0"/>
-          <a:ext cx="5115639" cy="4330395"/>
+          <a:off x="9357633" y="66675"/>
+          <a:ext cx="5115639" cy="4294336"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -586,16 +731,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>546440</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>32090</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>552495</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38145</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>33338</xdr:rowOff>
+      <xdr:rowOff>80963</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -618,7 +763,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8928440" y="0"/>
+          <a:off x="9852365" y="228600"/>
           <a:ext cx="2292055" cy="2371726"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -950,18 +1095,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2B24AA-CEA2-4D28-9D15-0A3296A1F5B7}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="23.265625" customWidth="1"/>
+    <col min="3" max="3" width="30.796875" customWidth="1"/>
+    <col min="4" max="4" width="19.1328125" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
     <col min="8" max="8" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="41.65" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="27.75" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -990,30 +1136,30 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="171" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="81" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1047,7 +1193,9 @@
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1059,7 +1207,9 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.45">
-      <c r="A6" s="2"/>
+      <c r="A6" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1073,7 +1223,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{32A72DAF-BD53-4E22-8FD3-32820F2D956D}"/>
+    <hyperlink ref="B2" r:id="rId1" display="Wrist‑based health sensor band reference platform lastminuteengineers​" xr:uid="{32A72DAF-BD53-4E22-8FD3-32820F2D956D}"/>
     <hyperlink ref="D2" r:id="rId2" display="https://lastminuteengineers.com/max30100-pulse-oximeter-heart-rate-sensor-arduino-tutorial/" xr:uid="{CEE8766C-56BD-42C1-AF70-7F35452FC634}"/>
     <hyperlink ref="E2" r:id="rId3" display="https://lastminuteengineers.com/max30100-pulse-oximeter-heart-rate-sensor-arduino-tutorial/" xr:uid="{79F118F2-39F8-4EB0-9BA8-FECB0F5372BB}"/>
     <hyperlink ref="F2" r:id="rId4" display="https://lastminuteengineers.com/max30100-pulse-oximeter-heart-rate-sensor-arduino-tutorial/" xr:uid="{AFA5C87B-243F-4509-AAE6-333A946C8F53}"/>
@@ -1091,7 +1241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25FD5D16-9CE2-4538-B176-6B687810665F}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -1137,28 +1287,28 @@
     </row>
     <row r="2" spans="1:11" ht="171" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1184,7 +1334,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1226,28 +1376,28 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1268,15 +1418,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93B2A36-3368-4BD8-9F26-B93066109403}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A2" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="22.19921875" customWidth="1"/>
+    <col min="3" max="3" width="18.796875" customWidth="1"/>
+    <col min="4" max="4" width="19.86328125" customWidth="1"/>
+    <col min="5" max="5" width="19.19921875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="20.86328125" customWidth="1"/>
+    <col min="8" max="8" width="17.59765625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="41.65" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="27.75" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1302,40 +1461,106 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="17" spans="1:8" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1346,10 +1571,24 @@
     <hyperlink ref="F2" r:id="rId5" display="https://easyelecmodule.com/max30100-max30102-pulse-oximeter-and-heart-rate-sensor-module/" xr:uid="{0F54D437-D603-4862-B17C-E0599B011302}"/>
     <hyperlink ref="G2" r:id="rId6" display="https://easyelecmodule.com/max30100-max30102-pulse-oximeter-and-heart-rate-sensor-module/" xr:uid="{981F1CFB-D0C4-48AD-B0CB-D4D2504D281F}"/>
     <hyperlink ref="H2" r:id="rId7" display="https://easyelecmodule.com/max30100-max30102-pulse-oximeter-and-heart-rate-sensor-module/" xr:uid="{7975AACC-4026-4900-ACA5-FF0BC00595CC}"/>
-    <hyperlink ref="B2:H3" r:id="rId8" display="Optical data‑acquisition EV kit easyelecmodule​" xr:uid="{9CCC8800-AA47-4BDD-A65A-28D7023077D1}"/>
+    <hyperlink ref="B2:H5" r:id="rId8" display="Optical data‑acquisition EV kit easyelecmodule​" xr:uid="{9CCC8800-AA47-4BDD-A65A-28D7023077D1}"/>
+    <hyperlink ref="B5" r:id="rId9" display="https://www.analog.com/media/en/technical-documentation/data-sheets/max30110.pdf" xr:uid="{4DFD55BF-D6C5-49A6-8E9B-73CED2532AE2}"/>
+    <hyperlink ref="C5" r:id="rId10" display="https://www.analog.com/media/en/technical-documentation/data-sheets/max30110.pdf" xr:uid="{ED856684-9420-471A-8660-FCA0A7CBE4BB}"/>
+    <hyperlink ref="D5" r:id="rId11" display="https://www.analog.com/media/en/technical-documentation/data-sheets/max30110.pdf" xr:uid="{BF730F77-3979-4DDB-B654-4D71D4893224}"/>
+    <hyperlink ref="E5" r:id="rId12" display="https://www.analog.com/media/en/technical-documentation/data-sheets/max30110.pdf" xr:uid="{B2EA2770-7F28-46B9-9D18-BBA6FB4DE354}"/>
+    <hyperlink ref="F5" r:id="rId13" display="https://www.analog.com/media/en/technical-documentation/data-sheets/max30110.pdf" xr:uid="{6BD1CF61-853A-4C60-85B8-FFA9CD758F51}"/>
+    <hyperlink ref="G5" r:id="rId14" display="https://uk.farnell.com/analog-devices/max30110accevkit/eval-board-optical-data-acquisition/dp/2775883" xr:uid="{1CCFF416-1C45-492A-A036-3E224656B6B6}"/>
+    <hyperlink ref="H5" r:id="rId15" display="https://www.analog.com/media/en/technical-documentation/data-sheets/max30110.pdf" xr:uid="{C8199001-081B-46E6-A987-97AA02E4BCDA}"/>
+    <hyperlink ref="B17" r:id="rId16" display="https://www.lisleapex.com/product-max30110ewg-" xr:uid="{7A9C28BF-0F8D-4830-BFB1-64D2EFEA4EAA}"/>
+    <hyperlink ref="C17" r:id="rId17" display="https://www.lisleapex.com/product-max30110ewg-" xr:uid="{7798CDFC-0C72-4E87-8760-7205430ED701}"/>
+    <hyperlink ref="D17" r:id="rId18" display="https://www.lisleapex.com/product-max30110ewg-" xr:uid="{848E8639-D6AC-44B5-92BE-1FAC5A821D0D}"/>
+    <hyperlink ref="E17" r:id="rId19" display="https://www.lisleapex.com/product-max30110ewg-" xr:uid="{1AC5BA98-A821-4A76-84F8-08A11BDFE6C1}"/>
+    <hyperlink ref="F17" r:id="rId20" display="https://www.lisleapex.com/product-max30110ewg-" xr:uid="{748DC5FE-2802-4678-8666-1FA82F51A067}"/>
+    <hyperlink ref="G17" r:id="rId21" display="https://uk.farnell.com/analog-devices/max30110accevkit/eval-board-optical-data-acquisition/dp/2775883" xr:uid="{33A6BFF5-5720-4D2C-ABEC-96EC81E1C0D6}"/>
+    <hyperlink ref="H17" r:id="rId22" display="https://www.lisleapex.com/product-max30110ewg-" xr:uid="{4F79CCC5-01F1-4317-89E7-D975AAD2C57A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId9"/>
+  <drawing r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -1357,11 +1596,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB5E59A-2059-493A-8767-E8B66F40525E}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="5" max="5" width="41.46484375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="41.65" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
@@ -1392,30 +1635,30 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="150" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1441,10 +1684,18 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="22.265625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" customWidth="1"/>
+    <col min="6" max="6" width="17.59765625" customWidth="1"/>
+    <col min="7" max="7" width="13.19921875" customWidth="1"/>
+    <col min="8" max="8" width="13.9296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="41.65" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
@@ -1475,30 +1726,30 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="114" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>

</xml_diff>